<commit_message>
updates to scrum docs
</commit_message>
<xml_diff>
--- a/CLCMinesweeperApp/Planning and Design/Week 2/CST-247-RS-SprintBackLog-W2.xlsx
+++ b/CLCMinesweeperApp/Planning and Design/Week 2/CST-247-RS-SprintBackLog-W2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
   <si>
     <t>Project Title:FR1
 Release #:1
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1077,8 +1077,12 @@
       <c r="E21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="F21" s="9">
+        <v>2</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">

</xml_diff>